<commit_message>
Updated file locations and added updated wireframes Updated time card
</commit_message>
<xml_diff>
--- a/RAW Files/time_cards.xlsx
+++ b/RAW Files/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Code/CSI-3471/Project/C.A.R./Iteration-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./RAW Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEFCAE0-C155-414F-9F1B-3864AC2A47D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE28C9AD-B8F0-C143-B895-D10B00BD94B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -72,14 +72,17 @@
     <t>8h 17m</t>
   </si>
   <si>
-    <t>Iteration 1 Timecards</t>
+    <t>Iteration 2 Tomecards</t>
+  </si>
+  <si>
+    <t>10h 30m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,19 +447,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,15 +469,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -480,7 +485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -488,7 +493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -496,7 +501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -504,7 +509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>

</xml_diff>